<commit_message>
feat: v0.0.15 + v2.2.9 Up_and_Down
</commit_message>
<xml_diff>
--- a/docs/03_strategies/DCA_Conditional_Buy_LR_with_TrailingStop/Up_and_down/Binance_BTC-USDT_1w/equity_curve.xlsx
+++ b/docs/03_strategies/DCA_Conditional_Buy_LR_with_TrailingStop/Up_and_down/Binance_BTC-USDT_1w/equity_curve.xlsx
@@ -400,7 +400,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -408,7 +408,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -416,7 +416,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -424,7 +424,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -432,7 +432,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -440,7 +440,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -448,7 +448,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -456,7 +456,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -464,23 +464,26 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>1600</v>
+        <v>995.0329786537201</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>0.00496702134627991</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>1600</v>
+        <v>1105.74449373372</v>
       </c>
       <c r="B11">
         <v>0</v>
+      </c>
+      <c r="C11" s="2">
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>1600</v>
+        <v>1174.98290685372</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -488,23 +491,26 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>1600</v>
+        <v>1163.36545365372</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>0.009887338047417704</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>1600</v>
+        <v>1259.37492761372</v>
       </c>
       <c r="B14">
         <v>0</v>
+      </c>
+      <c r="C14" s="2">
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15">
-        <v>1600</v>
+        <v>1369.28380665372</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -512,87 +518,90 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
-        <v>1600</v>
+        <v>1337.86442457372</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>0.02294585090930357</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17">
-        <v>1600</v>
+        <v>1340.42776805372</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>0.02107381863407765</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18">
-        <v>1600</v>
+        <v>1194.525367683652</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>0.1276276241060247</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19">
-        <v>1600</v>
+        <v>1194.525367683652</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>0.1276276241060247</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
-        <v>1600</v>
+        <v>1194.525367683652</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>0.1276276241060247</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21">
-        <v>1600</v>
+        <v>1194.525367683652</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>0.1276276241060247</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22">
-        <v>1600</v>
+        <v>1194.525367683652</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>0.1276276241060247</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23">
-        <v>1600</v>
+        <v>1343.729449920652</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>0.01866257134488269</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24">
-        <v>1629.05622830194</v>
+        <v>1365.781839180652</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>0.002557517627865491</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25">
-        <v>1679.79584345194</v>
+        <v>1402.300164880652</v>
       </c>
       <c r="B25">
         <v>0</v>
+      </c>
+      <c r="C25" s="2">
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26">
-        <v>1813.65768317194</v>
+        <v>1498.643234240652</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -600,7 +609,7 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27">
-        <v>2094.55799279194</v>
+        <v>1700.812859800652</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -608,15 +617,15 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28">
-        <v>2054.473813761941</v>
+        <v>1671.963466660653</v>
       </c>
       <c r="B28">
-        <v>0.01913729730470215</v>
+        <v>0.01696212077287629</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29">
-        <v>2278.35724955194</v>
+        <v>1833.096896680653</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -627,23 +636,23 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30">
-        <v>2053.90549265194</v>
+        <v>1671.554434480652</v>
       </c>
       <c r="B30">
-        <v>0.09851473334313154</v>
+        <v>0.08812543542707385</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31">
-        <v>2224.15157726194</v>
+        <v>1794.083979660652</v>
       </c>
       <c r="B31">
-        <v>0.02379155959876778</v>
+        <v>0.0212825176293977</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32">
-        <v>2294.01531470194</v>
+        <v>1844.366322380652</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -654,55 +663,55 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33">
-        <v>2199.32085617194</v>
+        <v>1776.212808240653</v>
       </c>
       <c r="B33">
-        <v>0.04127891297112107</v>
+        <v>0.03695226556296549</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34">
-        <v>2188.23274760194</v>
+        <v>1768.232472580652</v>
       </c>
       <c r="B34">
-        <v>0.04611240667054761</v>
+        <v>0.04127913683748508</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35">
-        <v>2146.52312342194</v>
+        <v>1738.213213740652</v>
       </c>
       <c r="B35">
-        <v>0.06429433593348244</v>
+        <v>0.05755532800175012</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36">
-        <v>2135.54493704194</v>
+        <v>1730.311991300652</v>
       </c>
       <c r="B36">
-        <v>0.06907991269473734</v>
+        <v>0.06183930474981902</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37">
-        <v>2190.11779622194</v>
+        <v>1769.589180140652</v>
       </c>
       <c r="B37">
-        <v>0.04529068215636545</v>
+        <v>0.04054354134133187</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38">
-        <v>2168.18948870194</v>
+        <v>1753.806934380652</v>
       </c>
       <c r="B38">
-        <v>0.05484960156700114</v>
+        <v>0.04910054304348221</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39">
-        <v>2337.17731505194</v>
+        <v>1875.430885680652</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -713,7 +722,7 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40">
-        <v>2603.75265842194</v>
+        <v>2067.290543740653</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -721,7 +730,7 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41">
-        <v>2746.49480783194</v>
+        <v>2170.024951320652</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -729,7 +738,7 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42">
-        <v>2800.12748147194</v>
+        <v>2208.625469640652</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -737,90 +746,90 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43">
-        <v>2738.64823448194</v>
+        <v>2164.377614020652</v>
       </c>
       <c r="B43">
-        <v>0.02195587429386681</v>
+        <v>0.02003411453332515</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44">
-        <v>2753.38950179194</v>
+        <v>2174.987201800653</v>
       </c>
       <c r="B44">
-        <v>0.01669137565673651</v>
+        <v>0.01523040837044798</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45">
-        <v>2413.10782187194</v>
+        <v>2105.722088421733</v>
       </c>
       <c r="B45">
-        <v>0.1382150141951949</v>
+        <v>0.04659159401782242</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46">
-        <v>2431.02981638194</v>
+        <v>2105.722088421733</v>
       </c>
       <c r="B46">
-        <v>0.1318145932755806</v>
+        <v>0.04659159401782242</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47">
-        <v>2568.420860031941</v>
+        <v>2105.722088421733</v>
       </c>
       <c r="B47">
-        <v>0.0827485973310752</v>
+        <v>0.04659159401782242</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48">
-        <v>2534.26780172194</v>
+        <v>2091.493446887773</v>
       </c>
       <c r="B48">
-        <v>0.09494556283924804</v>
+        <v>0.05303390020759702</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49">
-        <v>2509.09795898194</v>
+        <v>2070.857365117673</v>
       </c>
       <c r="B49">
-        <v>0.1039343831363758</v>
+        <v>0.06237730498752003</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50">
-        <v>2673.37082501194</v>
+        <v>2199.073040497673</v>
       </c>
       <c r="B50">
-        <v>0.04526817343093525</v>
+        <v>0.004325056137532202</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51">
-        <v>2704.73840825194</v>
+        <v>2223.555573537673</v>
       </c>
       <c r="B51">
-        <v>0.03406597515690846</v>
+        <v>0</v>
+      </c>
+      <c r="C51" s="2">
+        <v>63</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52">
-        <v>3061.56220838194</v>
+        <v>2502.058077517673</v>
       </c>
       <c r="B52">
         <v>0</v>
-      </c>
-      <c r="C52" s="2">
-        <v>70</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53">
-        <v>3232.91686997194</v>
+        <v>2635.801124657673</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -828,7 +837,7 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54">
-        <v>3633.688497171941</v>
+        <v>2948.605095857673</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -836,7 +845,7 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55">
-        <v>3746.39382347194</v>
+        <v>3036.572085657673</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -844,7 +853,7 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56">
-        <v>4321.13017958194</v>
+        <v>3485.156272717672</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -852,15 +861,15 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57">
-        <v>4267.469440701941</v>
+        <v>3443.273836237673</v>
       </c>
       <c r="B57">
-        <v>0.01241821853309477</v>
+        <v>0.01201737689866633</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58">
-        <v>4542.136928271941</v>
+        <v>3657.652986457673</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -871,15 +880,15 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59">
-        <v>4499.007670701941</v>
+        <v>3623.990416237673</v>
       </c>
       <c r="B59">
-        <v>0.009495367103872998</v>
+        <v>0.009203325286634478</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60">
-        <v>5500.125185511941</v>
+        <v>4405.366923497673</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -890,7 +899,7 @@
     </row>
     <row r="61" spans="1:3">
       <c r="A61">
-        <v>6161.09433029194</v>
+        <v>4921.256171377672</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -898,7 +907,7 @@
     </row>
     <row r="62" spans="1:3">
       <c r="A62">
-        <v>7732.371228321941</v>
+        <v>6147.644518757674</v>
       </c>
       <c r="B62">
         <v>0</v>
@@ -906,7 +915,7 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63">
-        <v>8936.830762011941</v>
+        <v>7087.730342497673</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -914,31 +923,31 @@
     </row>
     <row r="64" spans="1:3">
       <c r="A64">
-        <v>8393.906355441941</v>
+        <v>6663.975518277673</v>
       </c>
       <c r="B64">
-        <v>0.06075133579543945</v>
+        <v>0.05978709738421994</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65">
-        <v>7559.267166771941</v>
+        <v>6012.536057457673</v>
       </c>
       <c r="B65">
-        <v>0.1541445319850581</v>
+        <v>0.1516979672030112</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66">
-        <v>7754.10541793194</v>
+        <v>6164.608146817673</v>
       </c>
       <c r="B66">
-        <v>0.1323428154315563</v>
+        <v>0.1302422850577435</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67">
-        <v>9087.838124601942</v>
+        <v>7205.592235637674</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -949,7 +958,7 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68">
-        <v>11375.64632630194</v>
+        <v>8991.236333837674</v>
       </c>
       <c r="B68">
         <v>0</v>
@@ -957,7 +966,7 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69">
-        <v>13440.96266036194</v>
+        <v>10603.22457659767</v>
       </c>
       <c r="B69">
         <v>0</v>
@@ -965,23 +974,23 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70">
-        <v>10570.61128829194</v>
+        <v>8362.903039377674</v>
       </c>
       <c r="B70">
-        <v>0.2135525143994936</v>
+        <v>0.2112868138400655</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71">
-        <v>11935.53850922194</v>
+        <v>9428.234580157674</v>
       </c>
       <c r="B71">
-        <v>0.1120027031679485</v>
+        <v>0.1108144025387632</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72">
-        <v>13805.74997234194</v>
+        <v>10887.94263567767</v>
       </c>
       <c r="B72">
         <v>0</v>
@@ -992,31 +1001,31 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73">
-        <v>13427.62933259194</v>
+        <v>10592.81785717767</v>
       </c>
       <c r="B73">
-        <v>0.0273886344825538</v>
+        <v>0.02710565148763133</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74">
-        <v>13059.52330598194</v>
+        <v>10305.50952711767</v>
       </c>
       <c r="B74">
-        <v>0.05405187460695504</v>
+        <v>0.05349340348758636</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75">
-        <v>13626.53002724194</v>
+        <v>10748.06070107767</v>
       </c>
       <c r="B75">
-        <v>0.01298154359299875</v>
+        <v>0.0128474165671697</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76">
-        <v>14047.60685558194</v>
+        <v>11076.71296871767</v>
       </c>
       <c r="B76">
         <v>0</v>
@@ -1027,151 +1036,151 @@
     </row>
     <row r="77" spans="1:3">
       <c r="A77">
-        <v>13146.61442324194</v>
+        <v>10494.94941648466</v>
       </c>
       <c r="B77">
-        <v>0.06413850000236754</v>
+        <v>0.05252131691739259</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78">
-        <v>11490.00750176194</v>
+        <v>10378.08303972466</v>
       </c>
       <c r="B78">
-        <v>0.1820665526956797</v>
+        <v>0.06307195383378172</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79">
-        <v>13246.76055464194</v>
+        <v>10502.01428828466</v>
       </c>
       <c r="B79">
-        <v>0.05700944717297374</v>
+        <v>0.05188350389290131</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80">
-        <v>13635.61147115194</v>
+        <v>10557.54710882429</v>
       </c>
       <c r="B80">
-        <v>0.02932851044776297</v>
+        <v>0.04687002916475191</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81">
-        <v>10838.36648531738</v>
+        <v>9954.351817215951</v>
       </c>
       <c r="B81">
-        <v>0.2284545975166825</v>
+        <v>0.101326192587227</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82">
-        <v>10518.08781406738</v>
+        <v>9353.833724715951</v>
       </c>
       <c r="B82">
-        <v>0.2512541159359166</v>
+        <v>0.1555406598390151</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83">
-        <v>10544.90460000738</v>
+        <v>9404.11482859595</v>
       </c>
       <c r="B83">
-        <v>0.2493451227375951</v>
+        <v>0.1510013074136158</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84">
-        <v>10554.42798611046</v>
+        <v>9412.02093835595</v>
       </c>
       <c r="B84">
-        <v>0.2486671861893286</v>
+        <v>0.1502875478549518</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85">
-        <v>10926.50026653296</v>
+        <v>9664.619004606591</v>
       </c>
       <c r="B85">
-        <v>0.2221806618832576</v>
+        <v>0.1274831232062301</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86">
-        <v>10389.68411325088</v>
+        <v>9307.834799078832</v>
       </c>
       <c r="B86">
-        <v>0.2603947263001279</v>
+        <v>0.1596934193956657</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87">
-        <v>10248.87848001088</v>
+        <v>9214.23462285883</v>
       </c>
       <c r="B87">
-        <v>0.2704181868573297</v>
+        <v>0.1681435955882188</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88">
-        <v>10340.60353395088</v>
+        <v>9275.208612428831</v>
       </c>
       <c r="B88">
-        <v>0.2638886010792686</v>
+        <v>0.1626388948938702</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89">
-        <v>10132.03403498331</v>
+        <v>9168.324954508831</v>
       </c>
       <c r="B89">
-        <v>0.2787359342308718</v>
+        <v>0.1722882970424909</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90">
-        <v>9632.547365453311</v>
+        <v>8910.308145478832</v>
       </c>
       <c r="B90">
-        <v>0.3142926432607465</v>
+        <v>0.1955819230269032</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91">
-        <v>10357.97833811331</v>
+        <v>9285.039637138831</v>
       </c>
       <c r="B91">
-        <v>0.2626517495399956</v>
+        <v>0.1617513549948257</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92">
-        <v>11455.26670402893</v>
+        <v>9873.362009658211</v>
       </c>
       <c r="B92">
-        <v>0.1845396285790075</v>
+        <v>0.1086379111256118</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93">
-        <v>12582.46197374562</v>
+        <v>10491.63365630979</v>
       </c>
       <c r="B93">
-        <v>0.1042985397369752</v>
+        <v>0.05282066205563274</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94">
-        <v>13491.44447259562</v>
+        <v>11061.20575170199</v>
       </c>
       <c r="B94">
-        <v>0.03959125484532799</v>
+        <v>0.001399983646725889</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95">
-        <v>14139.10647479562</v>
+        <v>11514.49190964549</v>
       </c>
       <c r="B95">
         <v>0</v>
@@ -1182,15 +1191,15 @@
     </row>
     <row r="96" spans="1:3">
       <c r="A96">
-        <v>14004.33937352562</v>
+        <v>11409.49776525739</v>
       </c>
       <c r="B96">
-        <v>0.009531514704287369</v>
+        <v>0.009118434856873359</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97">
-        <v>14858.88784517562</v>
+        <v>12068.98083390739</v>
       </c>
       <c r="B97">
         <v>0</v>
@@ -1201,74 +1210,74 @@
     </row>
     <row r="98" spans="1:3">
       <c r="A98">
-        <v>13220.25209065562</v>
+        <v>10634.3414653148</v>
       </c>
       <c r="B98">
-        <v>0.1102798386793149</v>
+        <v>0.1188699682546532</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99">
-        <v>13568.04378408562</v>
+        <v>10797.2394533748</v>
       </c>
       <c r="B99">
-        <v>0.0868735314876955</v>
+        <v>0.105372723516113</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100">
-        <v>12401.35733503562</v>
+        <v>10250.7891532748</v>
       </c>
       <c r="B100">
-        <v>0.165391282022356</v>
+        <v>0.1506499766346834</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101">
-        <v>13842.00361026562</v>
+        <v>10925.5562169348</v>
       </c>
       <c r="B101">
-        <v>0.06843609330022371</v>
+        <v>0.09474077659980851</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102">
-        <v>15688.58363833562</v>
+        <v>11922.12494747941</v>
       </c>
       <c r="B102">
-        <v>0</v>
-      </c>
-      <c r="C102" s="2">
-        <v>35</v>
+        <v>0.01216804371876978</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103">
-        <v>17652.47700002562</v>
+        <v>13106.48575918029</v>
       </c>
       <c r="B103">
         <v>0</v>
+      </c>
+      <c r="C103" s="2">
+        <v>42</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104">
-        <v>17459.18188379562</v>
+        <v>12977.94980624149</v>
       </c>
       <c r="B104">
-        <v>0.01095002793260802</v>
+        <v>0.00980704937238952</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105">
-        <v>17587.14187273562</v>
+        <v>13068.67571802653</v>
       </c>
       <c r="B105">
-        <v>0.003701187504161929</v>
+        <v>0.002884834413166448</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106">
-        <v>18151.43461720562</v>
+        <v>13473.13489587653</v>
       </c>
       <c r="B106">
         <v>0</v>
@@ -1279,7 +1288,7 @@
     </row>
     <row r="107" spans="1:3">
       <c r="A107">
-        <v>18793.41020763562</v>
+        <v>13933.27357752653</v>
       </c>
       <c r="B107">
         <v>0</v>
@@ -1287,82 +1296,82 @@
     </row>
     <row r="108" spans="1:3">
       <c r="A108">
-        <v>16821.58331519562</v>
+        <v>12841.66498559055</v>
       </c>
       <c r="B108">
-        <v>0.1049211862378687</v>
+        <v>0.0783454502534624</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109">
-        <v>16436.44541917562</v>
+        <v>12732.59379549055</v>
       </c>
       <c r="B109">
-        <v>0.1254144278456915</v>
+        <v>0.08617355967032791</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110">
-        <v>14281.24181791728</v>
+        <v>12094.70699474055</v>
       </c>
       <c r="B110">
-        <v>0.2400931145474109</v>
+        <v>0.1319551053495049</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111">
-        <v>14299.12574920728</v>
+        <v>12147.94714979055</v>
       </c>
       <c r="B111">
-        <v>0.2391415080485151</v>
+        <v>0.1281340252024911</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112">
-        <v>14099.08714540178</v>
+        <v>11874.87892324055</v>
       </c>
       <c r="B112">
-        <v>0.2497855902877367</v>
+        <v>0.1477323073312823</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113">
-        <v>14340.00159232178</v>
+        <v>12206.37068414055</v>
       </c>
       <c r="B113">
-        <v>0.2369664986881654</v>
+        <v>0.1239409305915997</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114">
-        <v>14024.2474186277</v>
+        <v>11854.83784835698</v>
       </c>
       <c r="B114">
-        <v>0.2537678226738352</v>
+        <v>0.1491706681566871</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115">
-        <v>13536.1009993477</v>
+        <v>11195.68132401251</v>
       </c>
       <c r="B115">
-        <v>0.2797421622900518</v>
+        <v>0.1964787555689415</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116">
-        <v>13644.7804668677</v>
+        <v>11342.21356593251</v>
       </c>
       <c r="B116">
-        <v>0.2739593125400983</v>
+        <v>0.1859620423855911</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117">
-        <v>13643.1965065712</v>
+        <v>11342.21356593251</v>
       </c>
       <c r="B117">
-        <v>0.2740435952902219</v>
+        <v>0.1859620423855911</v>
       </c>
       <c r="C117" s="2">
         <v>70</v>

</xml_diff>